<commit_message>
changed to fit the ontology email terry sent out
</commit_message>
<xml_diff>
--- a/assignment/ns_occupations.xlsx
+++ b/assignment/ns_occupations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1015c\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0FBB3B3-9A25-4999-B190-7FFDF382F37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA3F8C-1EEE-4253-8BCB-762DB50E3F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10260" xr2:uid="{E75CB52D-7F99-4B12-A846-9FBD7C2010BE}"/>
+    <workbookView xWindow="8565" yWindow="0" windowWidth="8790" windowHeight="10155" xr2:uid="{E75CB52D-7F99-4B12-A846-9FBD7C2010BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,85 +36,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
-  <si>
-    <t>Data Scientist</t>
-  </si>
-  <si>
-    <t>Job Title</t>
-  </si>
-  <si>
-    <t>Education Needed</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Median Income (Dollars)</t>
-  </si>
-  <si>
-    <t>Job Outlook %</t>
-  </si>
-  <si>
-    <t>Bachelor's</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>Actuary</t>
-  </si>
-  <si>
-    <t>Financial Analyst</t>
-  </si>
-  <si>
-    <t>Market Research Analyst</t>
-  </si>
-  <si>
-    <t>Mathematician</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Food and Beverage Serving and Related Worker</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>Restaurant</t>
-  </si>
-  <si>
-    <t>Lawyer</t>
-  </si>
-  <si>
     <t>Law Degree</t>
   </si>
   <si>
-    <t>Animal Care and Service Worker</t>
-  </si>
-  <si>
     <t>High School</t>
   </si>
   <si>
-    <t>Zoo</t>
+    <t>job</t>
+  </si>
+  <si>
+    <t>pay</t>
+  </si>
+  <si>
+    <t>edu</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>n_employed</t>
+  </si>
+  <si>
+    <t>outlook</t>
+  </si>
+  <si>
+    <t>change_employment</t>
+  </si>
+  <si>
+    <t>top_places</t>
+  </si>
+  <si>
+    <t>physical_work_environment</t>
+  </si>
+  <si>
+    <t>social_work_environment</t>
+  </si>
+  <si>
+    <t>data scientist</t>
+  </si>
+  <si>
+    <t>actuary</t>
+  </si>
+  <si>
+    <t>financial analyst</t>
+  </si>
+  <si>
+    <t>market research analyst</t>
+  </si>
+  <si>
+    <t>mathematician</t>
+  </si>
+  <si>
+    <t>lawyer</t>
+  </si>
+  <si>
+    <t>animal care and service worker</t>
+  </si>
+  <si>
+    <t>food and beverage serving and related worker</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>zoo</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>office, remote, outside</t>
+  </si>
+  <si>
+    <t>team or solo</t>
+  </si>
+  <si>
+    <t>On Job</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>VA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -142,9 +173,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE3FBE32-7002-4B38-8B42-885DBB78AAEB}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -494,9 +526,9 @@
     <col min="5" max="5" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -505,146 +537,308 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2">
         <v>108020</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>202900</v>
+      </c>
+      <c r="G2" s="2">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="H2" s="2">
+        <v>73100</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>120000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>30200</v>
+      </c>
+      <c r="G3">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>6600</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>99890</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>404800</v>
+      </c>
+      <c r="G4">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
+      <c r="H4">
+        <v>37900</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>74680</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>903400</v>
+      </c>
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
+      <c r="H5">
+        <v>74900</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>104860</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>34800</v>
+      </c>
+      <c r="G6">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
+      <c r="H6">
+        <v>3900</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>145760</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>859000</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
+      <c r="H7">
+        <v>44200</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>31830</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8">
+        <v>422500</v>
+      </c>
+      <c r="G8">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
+      <c r="H8">
+        <v>64300</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>29710</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>4942100</v>
+      </c>
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
+      <c r="H9">
+        <v>268400</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>